<commit_message>
feat(publipostage): Add "status_label" as string version of "status"
</commit_message>
<xml_diff>
--- a/publipostage/003vg9w96/liste_essais_cliniques_identifies_003vg9w96.xlsx
+++ b/publipostage/003vg9w96/liste_essais_cliniques_identifies_003vg9w96.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,40 +441,45 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>status_label</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>NCTId</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>eudraCT</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>completion_year</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>clinical_trial_title</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>acronym</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>results_1y</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>results_3y</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>results</t>
         </is>
@@ -488,32 +493,37 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>rouge</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>NCT00439582</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr">
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
         <is>
           <t>2005</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>Comparative Effect of 2 Different Sources of Trans Fatty Acid (Milk Fat vs Hydrogenated Oil)on Cardiovascular Risk Factors in Healthy Humans</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>TRANSFACT1</t>
         </is>
       </c>
-      <c r="G2" t="b">
-        <v>0</v>
-      </c>
       <c r="H2" t="b">
         <v>0</v>
       </c>
       <c r="I2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" t="b">
         <v>0</v>
       </c>
     </row>
@@ -525,28 +535,33 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>rouge</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>NCT00873951</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr">
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
         <is>
           <t>2008</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>Influence of Protein Hydrolysis on Dietary Protein Digestibility and Metabolism in Healthy Subjects</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="b">
-        <v>0</v>
-      </c>
+      <c r="G3" t="inlineStr"/>
       <c r="H3" t="b">
         <v>0</v>
       </c>
       <c r="I3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -558,32 +573,37 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>rouge</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>NCT00685581</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr">
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
         <is>
           <t>2008</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>Rationale, Study Design and Baseline Data of the TRANSQUAL Clinical Trial: A Study to Evaluate the Impact of Different Milk Fatty Acid Profiles on Cardiovascular Risk Factors in Healthy Volunteers; Focus on Trans Fatty Acids</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>TRANSQUAL WPC</t>
         </is>
       </c>
-      <c r="G4" t="b">
-        <v>0</v>
-      </c>
       <c r="H4" t="b">
         <v>0</v>
       </c>
       <c r="I4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" t="b">
         <v>0</v>
       </c>
     </row>
@@ -595,28 +615,33 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>rouge</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>NCT00617435</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr">
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
         <is>
           <t>2009</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr">
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
         <is>
           <t>Trans-Insulin</t>
         </is>
       </c>
-      <c r="G5" t="b">
-        <v>0</v>
-      </c>
       <c r="H5" t="b">
         <v>0</v>
       </c>
       <c r="I5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" t="b">
         <v>1</v>
       </c>
     </row>
@@ -628,91 +653,106 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>rouge</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>NCT00931151</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr">
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
         <is>
           <t>2009</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
-      <c r="G6" t="b">
-        <v>0</v>
-      </c>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="b">
         <v>0</v>
       </c>
       <c r="I6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>🟥</t>
+          <t>🟧</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>NCT01209572</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr">
+          <t>orange</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>NCT00862329</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
         <is>
           <t>2010</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Modelling of 24h Energy Expenditure From Heart Rate, Actimetry and Other Parameters Recorded Under Free-living Conditions</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Modelheart</t>
-        </is>
-      </c>
-      <c r="G7" t="b">
-        <v>0</v>
-      </c>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
       <c r="H7" t="b">
         <v>0</v>
       </c>
       <c r="I7" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J7" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>🟧</t>
+          <t>🟥</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>NCT00862329</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr">
+          <t>rouge</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>NCT00690781</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
         <is>
           <t>2010</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="b">
-        <v>0</v>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Effect of Milk Proteins and Protein Feeding Pattern on Body Composition and Protein Metabolism in Energy Restricted Obese Subjects</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>SURPROL-CF-H</t>
+        </is>
       </c>
       <c r="H8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="J8" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -723,32 +763,37 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>NCT00690781</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr">
+          <t>rouge</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>NCT01209572</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
         <is>
           <t>2010</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Effect of Milk Proteins and Protein Feeding Pattern on Body Composition and Protein Metabolism in Energy Restricted Obese Subjects</t>
-        </is>
-      </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>SURPROL-CF-H</t>
-        </is>
-      </c>
-      <c r="G9" t="b">
-        <v>0</v>
+          <t>Modelling of 24h Energy Expenditure From Heart Rate, Actimetry and Other Parameters Recorded Under Free-living Conditions</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Modelheart</t>
+        </is>
       </c>
       <c r="H9" t="b">
         <v>0</v>
       </c>
       <c r="I9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" t="b">
         <v>0</v>
       </c>
     </row>
@@ -760,32 +805,37 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>rouge</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
           <t>NCT00994526</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr">
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
         <is>
           <t>2010</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>Effect of Processed Meat on Colorectal Carcinogenesis. Study of Mechanisms. Choice of Preventive Strategies</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>Hemcancer</t>
         </is>
       </c>
-      <c r="G10" t="b">
-        <v>0</v>
-      </c>
       <c r="H10" t="b">
         <v>0</v>
       </c>
       <c r="I10" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" t="b">
         <v>1</v>
       </c>
     </row>
@@ -797,28 +847,33 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>rouge</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
           <t>NCT01995162</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr">
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
         <is>
           <t>2013</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>A Smartphone Application to Evaluate Energy Expenditure and Duration of Moderate-intensity Activities in Free-living Conditions (eMouve 2)</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="b">
-        <v>0</v>
-      </c>
+      <c r="G11" t="inlineStr"/>
       <c r="H11" t="b">
         <v>0</v>
       </c>
       <c r="I11" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" t="b">
         <v>0</v>
       </c>
     </row>
@@ -830,28 +885,33 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>rouge</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
           <t>NCT01995253</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr">
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr">
         <is>
           <t>2013</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>A Smartphone Application to Evaluate Energy Expenditure and Duration of Moderate-intensity Activities</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="b">
-        <v>0</v>
-      </c>
+      <c r="G12" t="inlineStr"/>
       <c r="H12" t="b">
         <v>0</v>
       </c>
       <c r="I12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" t="b">
         <v>0</v>
       </c>
     </row>
@@ -863,94 +923,109 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>NCT02157805</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr">
+          <t>rouge</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>NCT02473302</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr">
         <is>
           <t>2014</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Effect of Technological Processes on Nutritional Quality of Meat Proteins</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="b">
-        <v>0</v>
-      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Preventive Strategies in Colorectal Carcinogenesis Production and Meat Processing</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr"/>
       <c r="H13" t="b">
         <v>0</v>
       </c>
       <c r="I13" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="J13" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>🟥</t>
+          <t>🟧</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>NCT02473302</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr">
+          <t>orange</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>NCT02354794</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr">
         <is>
           <t>2014</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Preventive Strategies in Colorectal Carcinogenesis Production and Meat Processing</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="b">
-        <v>0</v>
-      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Effect of Oral Supplementation With One Form of L-arginine on Vascular Endothelial Function in Healthy Subjects Featuring Risk Factors Related to the Metabolic Syndrome.</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr"/>
       <c r="H14" t="b">
         <v>0</v>
       </c>
       <c r="I14" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J14" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>🟧</t>
+          <t>🟥</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>NCT02354794</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr">
+          <t>rouge</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>NCT02157805</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr">
         <is>
           <t>2014</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>Effect of Oral Supplementation With One Form of L-arginine on Vascular Endothelial Function in Healthy Subjects Featuring Risk Factors Related to the Metabolic Syndrome.</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="b">
-        <v>0</v>
-      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Effect of Technological Processes on Nutritional Quality of Meat Proteins</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr"/>
       <c r="H15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" t="b">
         <v>1</v>
       </c>
     </row>
@@ -962,32 +1037,37 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
+          <t>rouge</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
           <t>NCT02348554</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr">
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr">
         <is>
           <t>2014</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>A Smartphone Application to Evaluate Energy Expenditure and Duration of Activities in Free-living Conditions for Overweight and Obese People (eMouve3)</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t>eMouve3</t>
         </is>
       </c>
-      <c r="G16" t="b">
-        <v>0</v>
-      </c>
       <c r="H16" t="b">
         <v>0</v>
       </c>
       <c r="I16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" t="b">
         <v>0</v>
       </c>
     </row>
@@ -999,32 +1079,37 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
+          <t>orange</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
           <t>NCT03492593</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr">
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr">
         <is>
           <t>2016</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="F17" t="inlineStr">
         <is>
           <t>Métabolismes Des caroténoïdes Dans la lumière du Tube Digestif de l'Homme Sain</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="G17" t="inlineStr">
         <is>
           <t>CarotenoiDig</t>
         </is>
       </c>
-      <c r="G17" t="b">
-        <v>0</v>
-      </c>
       <c r="H17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17" t="b">
+        <v>1</v>
+      </c>
+      <c r="J17" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1036,32 +1121,37 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
+          <t>rouge</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
           <t>NCT03265392</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr">
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr">
         <is>
           <t>2018</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="F18" t="inlineStr">
         <is>
           <t>Digestion: Building a Better Health and Better Understanding the Digestive Processes Thanks to Magnetic Resonance Imaging</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="G18" t="inlineStr">
         <is>
           <t>DECOUVRIR-M</t>
         </is>
       </c>
-      <c r="G18" t="b">
-        <v>0</v>
-      </c>
       <c r="H18" t="b">
         <v>0</v>
       </c>
       <c r="I18" t="b">
+        <v>0</v>
+      </c>
+      <c r="J18" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1073,28 +1163,33 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
+          <t>orange</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
           <t>NCT03279211</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr">
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr">
         <is>
           <t>2019</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="F19" t="inlineStr">
         <is>
           <t>True Ileal Amino Acid Digestibility of Whey and Zein Proteins in Healthy Volunteers With Naso-ileal Tubes</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="b">
-        <v>0</v>
-      </c>
+      <c r="G19" t="inlineStr"/>
       <c r="H19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J19" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1106,32 +1201,37 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
+          <t>orange</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
           <t>NCT04072770</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr">
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr">
         <is>
           <t>2020</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="F20" t="inlineStr">
         <is>
           <t>Bioavailability of Protein and Amino Acids of Pea Protein Isolate in Healthy Volunteers</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="G20" t="inlineStr">
         <is>
           <t>Qualipois</t>
         </is>
       </c>
-      <c r="G20" t="b">
-        <v>0</v>
-      </c>
       <c r="H20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20" t="b">
+        <v>1</v>
+      </c>
+      <c r="J20" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1143,32 +1243,37 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>NCT05047757</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr">
+          <t>rouge</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>NCT06624033</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr">
         <is>
           <t>2023</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Fava Bean Protein and Amino Acid Bioavailability in Healthy Volunteers</t>
-        </is>
-      </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Leg4Life</t>
-        </is>
-      </c>
-      <c r="G21" t="b">
-        <v>0</v>
+          <t>Single-blind, Randomized, Cross-over Comparative Bioavailability Study About the Kinetics of Plasma Amino Acid Concentrations Subsequent to the Consumption of Innovative Legume-based Products.</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>LEG'UP</t>
+        </is>
       </c>
       <c r="H21" t="b">
         <v>0</v>
       </c>
       <c r="I21" t="b">
+        <v>0</v>
+      </c>
+      <c r="J21" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1180,32 +1285,37 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>NCT06624033</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr">
+          <t>rouge</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>NCT05047757</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr">
         <is>
           <t>2023</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>Single-blind, Randomized, Cross-over Comparative Bioavailability Study About the Kinetics of Plasma Amino Acid Concentrations Subsequent to the Consumption of Innovative Legume-based Products.</t>
-        </is>
-      </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>LEG'UP</t>
-        </is>
-      </c>
-      <c r="G22" t="b">
-        <v>0</v>
+          <t>Fava Bean Protein and Amino Acid Bioavailability in Healthy Volunteers</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Leg4Life</t>
+        </is>
       </c>
       <c r="H22" t="b">
         <v>0</v>
       </c>
       <c r="I22" t="b">
+        <v>0</v>
+      </c>
+      <c r="J22" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1217,20 +1327,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
+          <t>rouge</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
           <t>NCT01154608</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
-      <c r="G23" t="b">
-        <v>0</v>
-      </c>
+      <c r="G23" t="inlineStr"/>
       <c r="H23" t="b">
         <v>0</v>
       </c>
       <c r="I23" t="b">
+        <v>0</v>
+      </c>
+      <c r="J23" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1242,24 +1357,29 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
+          <t>rouge</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
           <t>NCT02352740</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr">
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr">
         <is>
           <t>Characterization of the Metabolic Fate of an Oral L-arginine Form in Healthy Subjects Featuring Risk Factors Related to the Metabolic Syndrome.</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="b">
-        <v>0</v>
-      </c>
+      <c r="G24" t="inlineStr"/>
       <c r="H24" t="b">
         <v>0</v>
       </c>
       <c r="I24" t="b">
+        <v>0</v>
+      </c>
+      <c r="J24" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1271,24 +1391,29 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
+          <t>rouge</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
           <t>NCT00862017</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr">
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr">
         <is>
           <t>Effect of Monosodium Glutamate on Gastric Emptying and Postprandial Nitrogen in Healthy Volunteers</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="b">
-        <v>0</v>
-      </c>
+      <c r="G25" t="inlineStr"/>
       <c r="H25" t="b">
         <v>0</v>
       </c>
       <c r="I25" t="b">
+        <v>0</v>
+      </c>
+      <c r="J25" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1300,20 +1425,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
+          <t>rouge</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
           <t>NCT01154582</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
-      <c r="G26" t="b">
-        <v>0</v>
-      </c>
+      <c r="G26" t="inlineStr"/>
       <c r="H26" t="b">
         <v>0</v>
       </c>
       <c r="I26" t="b">
+        <v>0</v>
+      </c>
+      <c r="J26" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>